<commit_message>
temporal graphs added miRNA/mRNA
</commit_message>
<xml_diff>
--- a/comparison/comparison_tables.xlsx
+++ b/comparison/comparison_tables.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beyzakaya/Desktop/temporalHiC/comparison/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A412ABF-721C-C745-BF14-B3E1A35A9673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E916571C-4D95-144A-B28C-CC6F251817BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="640" yWindow="6340" windowWidth="33980" windowHeight="17240" xr2:uid="{960A1F96-E8F3-A04D-9C7E-C46B95EF2BE9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Comparison Tables" sheetId="1" r:id="rId1"/>
+    <sheet name="Comparison Tables mRNA)" sheetId="3" r:id="rId1"/>
+    <sheet name="Comparison Tables miRNA" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="54">
   <si>
     <t>Node2Vec Parameters</t>
   </si>
@@ -640,10 +641,256 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ABFF144-D7B4-5647-BADF-BDDFF9ACED1F}">
+  <dimension ref="C4:O21"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="39.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="41.5" customWidth="1"/>
+    <col min="14" max="14" width="20" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="C4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="3:15" ht="36" x14ac:dyDescent="0.2">
+      <c r="C5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="H5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="M5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+    </row>
+    <row r="6" spans="3:15" ht="36" x14ac:dyDescent="0.2">
+      <c r="C6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="H6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="M6" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+    </row>
+    <row r="7" spans="3:15" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="H7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="M7" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+    </row>
+    <row r="8" spans="3:15" ht="54" x14ac:dyDescent="0.2">
+      <c r="C8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="H8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="M8" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+    </row>
+    <row r="9" spans="3:15" ht="72" x14ac:dyDescent="0.2">
+      <c r="C9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="H9" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="M9" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+    </row>
+    <row r="10" spans="3:15" ht="36" x14ac:dyDescent="0.2">
+      <c r="C10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="M10" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+    </row>
+    <row r="11" spans="3:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="C11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="M11" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+    </row>
+    <row r="12" spans="3:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="C12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="M12" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+    </row>
+    <row r="13" spans="3:15" ht="54" x14ac:dyDescent="0.2">
+      <c r="C13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="M13" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+    </row>
+    <row r="14" spans="3:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="C14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="3:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="C15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+    </row>
+    <row r="16" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27B7D9BC-218D-F84A-BC35-66E4739E78CA}">
   <dimension ref="C4:O21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
miRNA best correl/worst correl gene tables
</commit_message>
<xml_diff>
--- a/comparison/comparison_tables.xlsx
+++ b/comparison/comparison_tables.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beyzakaya/Desktop/temporalHiC/comparison/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E916571C-4D95-144A-B28C-CC6F251817BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1572FC3-76E8-2845-B5FF-319C2774B997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="6340" windowWidth="33980" windowHeight="17240" xr2:uid="{960A1F96-E8F3-A04D-9C7E-C46B95EF2BE9}"/>
+    <workbookView xWindow="4860" yWindow="6240" windowWidth="33980" windowHeight="17240" xr2:uid="{960A1F96-E8F3-A04D-9C7E-C46B95EF2BE9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Comparison Tables mRNA)" sheetId="3" r:id="rId1"/>
+    <sheet name="Comparison Tables mRNA" sheetId="3" r:id="rId1"/>
     <sheet name="Comparison Tables miRNA" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -644,7 +644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ABFF144-D7B4-5647-BADF-BDDFF9ACED1F}">
   <dimension ref="C4:O21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
@@ -890,8 +890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27B7D9BC-218D-F84A-BC35-66E4739E78CA}">
   <dimension ref="C4:O21"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
comparison models for mRNA/miRNA done
</commit_message>
<xml_diff>
--- a/comparison/comparison_tables.xlsx
+++ b/comparison/comparison_tables.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beyzakaya/Desktop/temporalHiC/comparison/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A76CC8C-6C3C-F54F-B7BE-24B29902DCFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{568B810C-98B9-2548-A553-016108BBEC20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10240" yWindow="7080" windowWidth="33980" windowHeight="17240" activeTab="1" xr2:uid="{960A1F96-E8F3-A04D-9C7E-C46B95EF2BE9}"/>
+    <workbookView xWindow="9240" yWindow="9860" windowWidth="31500" windowHeight="17840" activeTab="1" xr2:uid="{960A1F96-E8F3-A04D-9C7E-C46B95EF2BE9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Comparison Tables mRNA" sheetId="3" r:id="rId1"/>
-    <sheet name="Comparison Tables miRNA" sheetId="1" r:id="rId2"/>
+    <sheet name="Comparison Tables miRNA" sheetId="1" r:id="rId1"/>
+    <sheet name="Comparison Tables mRNA " sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="54">
   <si>
     <t>Node2Vec Parameters</t>
   </si>
@@ -199,15 +199,6 @@
   </si>
   <si>
     <t>0.63</t>
-  </si>
-  <si>
-    <t>0.29</t>
-  </si>
-  <si>
-    <t>0.19</t>
-  </si>
-  <si>
-    <t>0.15</t>
   </si>
 </sst>
 </file>
@@ -650,11 +641,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ABFF144-D7B4-5647-BADF-BDDFF9ACED1F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27B7D9BC-218D-F84A-BC35-66E4739E78CA}">
   <dimension ref="C4:O21"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView showGridLines="0" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -703,47 +694,79 @@
       <c r="C5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="H5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+      <c r="I5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="M5" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
+      <c r="N5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="6" spans="3:15" ht="36" x14ac:dyDescent="0.2">
       <c r="C6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="H6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
+      <c r="I6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="M6" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-    </row>
-    <row r="7" spans="3:15" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="3:15" ht="72" x14ac:dyDescent="0.2">
       <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="D7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="H7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
+      <c r="I7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="M7" s="7" t="s">
         <v>42</v>
       </c>
@@ -754,13 +777,21 @@
       <c r="C8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="H8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
+      <c r="I8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="M8" s="7" t="s">
         <v>43</v>
       </c>
@@ -771,8 +802,12 @@
       <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="H9" s="8" t="s">
         <v>52</v>
       </c>
@@ -781,30 +816,46 @@
       <c r="M9" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
+      <c r="N9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="10" spans="3:15" ht="36" x14ac:dyDescent="0.2">
       <c r="C10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="D10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="H10" s="5"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
       <c r="M10" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
+      <c r="N10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="11" spans="3:15" ht="18" x14ac:dyDescent="0.2">
       <c r="C11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
@@ -818,8 +869,12 @@
       <c r="C12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
@@ -833,8 +888,12 @@
       <c r="C13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+      <c r="D13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
@@ -848,8 +907,12 @@
       <c r="C14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="D14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
@@ -858,8 +921,12 @@
       <c r="C15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -891,16 +958,17 @@
       <c r="D21" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27B7D9BC-218D-F84A-BC35-66E4739E78CA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61EC5C4B-1855-F443-91B7-3FD86D606C3D}">
   <dimension ref="C4:O21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -949,79 +1017,47 @@
       <c r="C5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
       <c r="H5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>28</v>
-      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
       <c r="M5" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="N5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>24</v>
-      </c>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
     </row>
     <row r="6" spans="3:15" ht="36" x14ac:dyDescent="0.2">
       <c r="C6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
       <c r="H6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>26</v>
-      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
       <c r="M6" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="N6" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="3:15" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+    </row>
+    <row r="7" spans="3:15" ht="72" x14ac:dyDescent="0.2">
       <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
       <c r="H7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>24</v>
-      </c>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
       <c r="M7" s="7" t="s">
         <v>42</v>
       </c>
@@ -1032,21 +1068,13 @@
       <c r="C8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
       <c r="H8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
       <c r="M8" s="7" t="s">
         <v>43</v>
       </c>
@@ -1057,12 +1085,8 @@
       <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
       <c r="H9" s="8" t="s">
         <v>52</v>
       </c>
@@ -1071,92 +1095,60 @@
       <c r="M9" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="N9" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="O9" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
     </row>
     <row r="10" spans="3:15" ht="36" x14ac:dyDescent="0.2">
       <c r="C10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>24</v>
-      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
       <c r="H10" s="5"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
       <c r="M10" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="N10" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="O10" s="3" t="s">
-        <v>50</v>
-      </c>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
     </row>
     <row r="11" spans="3:15" ht="18" x14ac:dyDescent="0.2">
       <c r="C11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
       <c r="M11" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="N11" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="O11" s="3" t="s">
-        <v>54</v>
-      </c>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
     </row>
     <row r="12" spans="3:15" ht="18" x14ac:dyDescent="0.2">
       <c r="C12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
       <c r="M12" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="N12" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="O12" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
     </row>
     <row r="13" spans="3:15" ht="54" x14ac:dyDescent="0.2">
       <c r="C13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
@@ -1170,12 +1162,8 @@
       <c r="C14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>28</v>
-      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
@@ -1184,12 +1172,8 @@
       <c r="C15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -1221,7 +1205,6 @@
       <c r="D21" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>